<commit_message>
1207 CL 10 experimental results
</commit_message>
<xml_diff>
--- a/BBT Tests/Results_Summary.xlsx
+++ b/BBT Tests/Results_Summary.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CL10_BBT_SummaryResults" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,22 +25,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>bending strain</t>
   </si>
   <si>
     <t>AUE</t>
   </si>
+  <si>
+    <t>Crit Bending strain</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>Critical bending strain</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -65,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -162,7 +180,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$14</c:f>
+              <c:f>CL10_BBT_SummaryResults!$B$3:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -175,12 +193,24 @@
                 <c:pt idx="2">
                   <c:v>0.1</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8000000000000003E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$14</c:f>
+              <c:f>CL10_BBT_SummaryResults!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -188,10 +218,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.4999999999999997E-2</c:v>
+                  <c:v>5.1799999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3199999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -383,7 +425,402 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.38808705161854767"/>
+                  <c:y val="-0.14266987459900854"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AC12-4BD7-A55F-8C82093EF600}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="371902608"/>
+        <c:axId val="371904248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="371902608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="371904248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="371904248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="371902608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -939,7 +1376,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1237,44 +2225,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="B4">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5.1400000000000001E-2</v>
+      </c>
+      <c r="B6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="B8">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5.3199999999999997E-2</v>
+      </c>
+      <c r="B9">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0.12</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0.122</v>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.09</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>-0.003*C5+0.12</f>
+        <v>0.06</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>-0.003*C6+0.12</f>
+        <v>0.105</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>-0.003*C7+0.12</f>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="B4">
-        <v>4.7E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0.1</v>
+      <c r="C7">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edits and postprocessing of data
</commit_message>
<xml_diff>
--- a/BBT Tests/Results_Summary.xlsx
+++ b/BBT Tests/Results_Summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CL15_BBT_SummaryResults" sheetId="4" r:id="rId1"/>
@@ -137,7 +137,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1130,44 +1129,8 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:intercept val="0.14000000000000001"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.2690605861767279"/>
-                  <c:y val="2.7629410906969961E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1212,7 +1175,7 @@
                   <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11750000000000002</c:v>
+                  <c:v>0.112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1256,6 +1219,56 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Corrosion Level (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1280,14 +1293,11 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1318,6 +1328,56 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Critical Bending Strain (in/in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1342,14 +1402,11 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1391,7 +1448,13 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1456,7 +1519,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-0.19148936170212755</c:v>
+                  <c:v>-0.25000000000000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1777,8 +1840,101 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="8"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CL=5%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$36:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.104</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$36:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.33E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-70FB-45A4-BCE3-7353590796E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>CL=10%</c:v>
           </c:tx>
@@ -1873,7 +2029,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>CL=15%</c:v>
           </c:tx>
@@ -1956,7 +2112,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>CL=20%</c:v>
           </c:tx>
@@ -2045,7 +2201,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:v>Pristine Condition</c:v>
           </c:tx>
@@ -2188,7 +2344,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:v>Critical Bending Strain CL10</c:v>
           </c:tx>
@@ -2244,7 +2400,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:v>Critical Bending CL15</c:v>
           </c:tx>
@@ -2300,7 +2456,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:order val="7"/>
           <c:tx>
             <c:v>Critical Bending Strain CL20</c:v>
           </c:tx>
@@ -2356,7 +2512,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
-          <c:order val="7"/>
+          <c:order val="8"/>
           <c:tx>
             <c:v>Critical Bending Strain Pristine</c:v>
           </c:tx>
@@ -2407,6 +2563,64 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-63E0-4E55-AB1B-B212E806F05F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Critical Bending Strain CL5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$11:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.112</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$11:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-70FB-45A4-BCE3-7353590796E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2676,10 +2890,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.1401356080489951E-2"/>
-          <c:y val="0.12904709827938174"/>
-          <c:w val="0.24134100258744254"/>
-          <c:h val="0.38079469233012542"/>
+          <c:x val="0.12922637329908226"/>
+          <c:y val="5.8434518115142157E-2"/>
+          <c:w val="0.24547420934085368"/>
+          <c:h val="0.44312311428361173"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -6254,16 +6468,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6793,8 +7007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6859,12 +7073,11 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <f>-0.0045*A7+0.14</f>
-        <v>0.11750000000000002</v>
+        <v>0.112</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>-0.19148936170212755</v>
+        <v>-0.25000000000000011</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6873,7 +7086,7 @@
       </c>
       <c r="B9" s="3">
         <f>+C7</f>
-        <v>-0.19148936170212755</v>
+        <v>-0.25000000000000011</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6911,10 +7124,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G35"/>
+  <dimension ref="A2:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7079,6 +7292,12 @@
       <c r="C11">
         <v>4.4999999999999998E-2</v>
       </c>
+      <c r="F11">
+        <v>0.112</v>
+      </c>
+      <c r="G11">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -7090,6 +7309,12 @@
       <c r="C12">
         <v>4.7E-2</v>
       </c>
+      <c r="F12">
+        <v>0.112</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -7342,6 +7567,72 @@
       </c>
       <c r="C35">
         <v>9.3770000000000006E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C36">
+        <v>5.33E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="C37">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>0.104</v>
+      </c>
+      <c r="C38">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>0.125</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>0.12</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit in figures and spectrum analysis of SEM
</commit_message>
<xml_diff>
--- a/BBT Tests/Results_Summary.xlsx
+++ b/BBT Tests/Results_Summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CL15_BBT_SummaryResults" sheetId="4" r:id="rId1"/>
@@ -137,6 +137,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -447,7 +448,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6768,9 +6768,9 @@
       <selection activeCell="A3" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>0</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4.7E-2</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>0</v>
       </c>
@@ -6818,7 +6818,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>4.7E-2</v>
       </c>
@@ -6841,9 +6841,9 @@
       <selection activeCell="A3" sqref="A3:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -6851,7 +6851,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>3.5299999999999998E-2</v>
       </c>
@@ -6867,7 +6867,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>0</v>
       </c>
@@ -6875,7 +6875,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>0</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>3.0700000000000002E-2</v>
       </c>
@@ -6899,7 +6899,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>3.6299999999999999E-2</v>
       </c>
@@ -6922,9 +6922,9 @@
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -6932,7 +6932,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>0</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>5.1799999999999999E-2</v>
       </c>
@@ -6956,7 +6956,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5.1400000000000001E-2</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>0</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>4.9200000000000001E-2</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>5.3199999999999997E-2</v>
       </c>
@@ -7007,16 +7007,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>0</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>10</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>-0.59090909090909116</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>20</v>
       </c>
@@ -7056,7 +7056,7 @@
         <v>-1.4561403508771933</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>15</v>
       </c>
@@ -7068,7 +7068,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>-0.25000000000000011</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>5</v>
       </c>
@@ -7089,7 +7089,7 @@
         <v>-0.25000000000000011</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>10</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>-0.59090909090909116</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>15</v>
       </c>
@@ -7107,7 +7107,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>20</v>
       </c>
@@ -7126,16 +7126,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>10</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>10</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>10</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>10</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>10</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>10</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>10</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>15</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>15</v>
       </c>
@@ -7299,7 +7299,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>15</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>15</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>15</v>
       </c>
@@ -7338,7 +7338,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>20</v>
       </c>
@@ -7349,7 +7349,7 @@
         <v>3.5299999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>20</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>20</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>20</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>20</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>3.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>20</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>0</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>0.1033</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>0</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v>0.11493</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>0</v>
       </c>
@@ -7437,7 +7437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>0</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>0</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>0.11466</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>0</v>
       </c>
@@ -7470,7 +7470,7 @@
         <v>5.1200000000000004E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>0</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>0.11358</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>0</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>0</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>0.16006999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>0</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>0.14873</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>0</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>0</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>0</v>
       </c>
@@ -7547,7 +7547,7 @@
         <v>0.17008000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>0</v>
       </c>
@@ -7558,7 +7558,7 @@
         <v>5.4879999999999998E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>0</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>9.3770000000000006E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>5</v>
       </c>
@@ -7580,7 +7580,7 @@
         <v>5.33E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>5</v>
       </c>
@@ -7591,7 +7591,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>5</v>
       </c>
@@ -7602,7 +7602,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>5</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>5</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Tests rults turned down bars
</commit_message>
<xml_diff>
--- a/BBT Tests/Results_Summary.xlsx
+++ b/BBT Tests/Results_Summary.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CL15_BBT_SummaryResults" sheetId="4" r:id="rId1"/>
     <sheet name="CL20_BBT_SummaryResults" sheetId="3" r:id="rId2"/>
     <sheet name="CL10_BBT_SummaryResults" sheetId="1" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="results_w_td_bars" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
   <si>
     <t>bending strain</t>
   </si>
@@ -49,6 +50,12 @@
   </si>
   <si>
     <t>crit bending strain</t>
+  </si>
+  <si>
+    <t>turned down</t>
+  </si>
+  <si>
+    <t>turned down - barcley et al.</t>
   </si>
 </sst>
 </file>
@@ -448,6 +455,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1843,6 +1851,1289 @@
           <c:idx val="8"/>
           <c:order val="0"/>
           <c:tx>
+            <c:v>Corroded Specimens</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$B$3:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.7000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.7000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.4000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.104</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.13100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$C$3:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3199999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5299999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.0700000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.6299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.33E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Pristine Condition</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="65000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$B$27:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>9.2170000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11927</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14434</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15254999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12021</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15776000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.13941999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15803</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10323</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.10879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.15556</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16444</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.14452999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.12684999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.10712000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$C$27:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.1033</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11493</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11466</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1200000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11358</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16006999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14873</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.17008000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.4879999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.3770000000000006E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Turned Down Corroded Specimens</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$B$42:$B$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.188</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.20699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.187</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$C$42:$C$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3000000000000004E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Turned Down - Barcley et al.</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$B$48:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.245</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$C$48:$C$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.11799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Critical Bending Strain CL10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$F$3:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$G$3:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Critical Bending CL15</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$F$5:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$G$5:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Critical Bending Strain CL20</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dashDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$F$7:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$G$7:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Critical Bending Strain Pristine</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$F$9:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$G$9:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>Critical Bending Strain CL5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="lgDashDotDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$F$11:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.112</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$G$11:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Critical Bending Strain - Turned Down Calderon</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$F$13:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$G$13:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:v>Turned Down - Barcley et al.</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$F$15:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.245</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.245</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results_w_td_bars!$G$15:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-87CB-4A98-B84F-CF17056E8C2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="399956176"/>
+        <c:axId val="399950272"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="399956176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Bending</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Strain </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" baseline="0">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>ε</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="-25000">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>b</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t> (in/in)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="399950272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="399950272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.18000000000000002"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Uniform Axial Elongation (in/in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="399956176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.60676774445747461"/>
+          <c:y val="5.0233352541788449E-2"/>
+          <c:w val="0.34949312187040443"/>
+          <c:h val="0.29586298177388187"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="0"/>
+          <c:tx>
             <c:v>CL=5%</c:v>
           </c:tx>
           <c:spPr>
@@ -3207,6 +4498,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5775,6 +7106,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6468,6 +8315,43 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>8</xdr:row>
@@ -6768,9 +8652,9 @@
       <selection activeCell="A3" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -6778,7 +8662,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6786,7 +8670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -6794,7 +8678,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -6802,7 +8686,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4.7E-2</v>
       </c>
@@ -6810,7 +8694,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -6818,7 +8702,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4.7E-2</v>
       </c>
@@ -6841,9 +8725,9 @@
       <selection activeCell="A3" sqref="A3:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -6851,7 +8735,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6859,7 +8743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3.5299999999999998E-2</v>
       </c>
@@ -6867,7 +8751,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -6875,7 +8759,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -6883,7 +8767,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -6891,7 +8775,7 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.0700000000000002E-2</v>
       </c>
@@ -6899,7 +8783,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.6299999999999999E-2</v>
       </c>
@@ -6922,9 +8806,9 @@
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -6932,7 +8816,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6940,7 +8824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -6948,7 +8832,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.1799999999999999E-2</v>
       </c>
@@ -6956,7 +8840,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -6964,7 +8848,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5.1400000000000001E-2</v>
       </c>
@@ -6972,7 +8856,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -6980,7 +8864,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.9200000000000001E-2</v>
       </c>
@@ -6988,7 +8872,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.3199999999999997E-2</v>
       </c>
@@ -7007,16 +8891,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7024,7 +8908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -7032,7 +8916,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -7044,7 +8928,7 @@
         <v>-0.59090909090909116</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20</v>
       </c>
@@ -7056,7 +8940,7 @@
         <v>-1.4561403508771933</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -7068,7 +8952,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7080,7 +8964,7 @@
         <v>-0.25000000000000011</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -7089,7 +8973,7 @@
         <v>-0.25000000000000011</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -7098,7 +8982,7 @@
         <v>-0.59090909090909116</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -7107,7 +8991,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20</v>
       </c>
@@ -7124,18 +9008,683 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0.122</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C4">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>5.1400000000000001E-2</v>
+      </c>
+      <c r="F6">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.06</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="C8">
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.06</v>
+      </c>
+      <c r="G8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="C9">
+        <v>5.3199999999999997E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0.08</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="C11">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.112</v>
+      </c>
+      <c r="G11">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="C12">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.112</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0.23</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.23</v>
+      </c>
+      <c r="G14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C15">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.245</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0.245</v>
+      </c>
+      <c r="G16">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C19">
+        <v>3.0700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C20">
+        <v>3.6299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C21">
+        <v>5.33E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="C22">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>0.104</v>
+      </c>
+      <c r="C23">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>0.125</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>0.12</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>9.2170000000000002E-2</v>
+      </c>
+      <c r="C27">
+        <v>0.1033</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0.11927</v>
+      </c>
+      <c r="C28">
+        <v>0.11493</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0.14434</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0.15254999999999999</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0.12021</v>
+      </c>
+      <c r="C31">
+        <v>0.11466</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0.15776000000000001</v>
+      </c>
+      <c r="C32">
+        <v>5.1200000000000004E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0.13941999999999999</v>
+      </c>
+      <c r="C33">
+        <v>0.11358</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0.15803</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>0.10323</v>
+      </c>
+      <c r="C35">
+        <v>0.16006999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>0.10879999999999999</v>
+      </c>
+      <c r="C36">
+        <v>0.14873</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0.15556</v>
+      </c>
+      <c r="C37">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>0.16444</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>0.14452999999999999</v>
+      </c>
+      <c r="C39">
+        <v>0.17008000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>0.12684999999999999</v>
+      </c>
+      <c r="C40">
+        <v>5.4879999999999998E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>0.10712000000000001</v>
+      </c>
+      <c r="C41">
+        <v>9.3770000000000006E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>0.17</v>
+      </c>
+      <c r="C42">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <v>0.23399999999999999</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45">
+        <v>0.188</v>
+      </c>
+      <c r="C45">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="C46">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>0.187</v>
+      </c>
+      <c r="C47">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>0.15</v>
+      </c>
+      <c r="C48">
+        <v>0.11799999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C49">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50">
+        <v>0.245</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="C51">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C52">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7146,7 +9695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -7163,7 +9712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -7180,7 +9729,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -7197,7 +9746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -7214,7 +9763,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -7231,7 +9780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -7248,7 +9797,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -7265,7 +9814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>15</v>
       </c>
@@ -7282,7 +9831,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -7299,7 +9848,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>15</v>
       </c>
@@ -7316,7 +9865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
@@ -7327,7 +9876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
@@ -7338,7 +9887,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20</v>
       </c>
@@ -7349,7 +9898,7 @@
         <v>3.5299999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20</v>
       </c>
@@ -7360,7 +9909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20</v>
       </c>
@@ -7371,7 +9920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20</v>
       </c>
@@ -7382,7 +9931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -7393,7 +9942,7 @@
         <v>3.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -7404,7 +9953,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -7415,7 +9964,7 @@
         <v>0.1033</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -7426,7 +9975,7 @@
         <v>0.11493</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -7437,7 +9986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -7448,7 +9997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -7459,7 +10008,7 @@
         <v>0.11466</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -7470,7 +10019,7 @@
         <v>5.1200000000000004E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -7481,7 +10030,7 @@
         <v>0.11358</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -7492,7 +10041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -7503,7 +10052,7 @@
         <v>0.16006999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -7514,7 +10063,7 @@
         <v>0.14873</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -7525,7 +10074,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -7536,7 +10085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -7547,7 +10096,7 @@
         <v>0.17008000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -7558,7 +10107,7 @@
         <v>5.4879999999999998E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0</v>
       </c>
@@ -7569,7 +10118,7 @@
         <v>9.3770000000000006E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -7580,7 +10129,7 @@
         <v>5.33E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5</v>
       </c>
@@ -7591,7 +10140,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>5</v>
       </c>
@@ -7602,7 +10151,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>5</v>
       </c>
@@ -7613,7 +10162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5</v>
       </c>
@@ -7624,7 +10173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
mores results from turned down bars
</commit_message>
<xml_diff>
--- a/BBT Tests/Results_Summary.xlsx
+++ b/BBT Tests/Results_Summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CL15_BBT_SummaryResults" sheetId="4" r:id="rId1"/>
@@ -2806,45 +2806,27 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Bending</a:t>
+                  <a:t>Bending Strain </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Strain </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="el-GR" baseline="0">
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
+                  <a:rPr lang="el-GR"/>
                   <a:t>ε</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="-25000">
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t>b</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>b (in/in)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0">
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> (in/in)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2862,13 +2844,13 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -2894,13 +2876,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2939,18 +2921,18 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Uniform Axial Elongation (in/in)</a:t>
+                  <a:t>Uniform Axial Elongation, UAE (in/in)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2969,13 +2951,13 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -3001,13 +2983,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3033,10 +3015,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.60676774445747461"/>
-          <c:y val="5.0233352541788449E-2"/>
-          <c:w val="0.34949312187040443"/>
-          <c:h val="0.29586298177388187"/>
+          <c:x val="0.64565669291338579"/>
+          <c:y val="5.0233205646591471E-2"/>
+          <c:w val="0.30782655293088362"/>
+          <c:h val="0.26461286089238845"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3060,9 +3042,9 @@
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3078,12 +3060,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -3093,10 +3070,12 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr>
+        <a:defRPr sz="1100">
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -3105,7 +3084,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -8322,9 +8301,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>125729</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9010,8 +8989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9667,7 +9646,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>